<commit_message>
add atlases, left and right eye check script, and images, orders for loc,
</commit_message>
<xml_diff>
--- a/Orders_LOC/PAR01_RUN01.xlsx
+++ b/Orders_LOC/PAR01_RUN01.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolcoricelli/Documents/GitHub/fMRI_3DReachspaces_CC_2021/Experiment/Orders_LOC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edeligia\Documents\GitHub\3D_Faces_ED\Orders_LOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7059ACA-20D1-5F49-82D4-1523598FDBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="25060" windowHeight="13600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="495" windowWidth="25065" windowHeight="13605"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -304,7 +303,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,7 +351,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -624,22 +623,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -667,13 +666,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -693,7 +692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -713,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -733,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -753,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -773,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -793,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -813,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -833,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -853,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -873,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -893,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -913,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -933,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -953,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -973,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -993,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1013,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -1033,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -1053,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -1073,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -1093,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -1133,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -1193,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -1213,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -1233,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -1253,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -1313,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2</v>
       </c>
@@ -1333,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>3</v>
       </c>
@@ -1353,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>3</v>
       </c>
@@ -1373,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3</v>
       </c>
@@ -1393,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>3</v>
       </c>
@@ -1413,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>3</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>3</v>
       </c>
@@ -1453,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>3</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>3</v>
       </c>
@@ -1493,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>3</v>
       </c>
@@ -1513,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>3</v>
       </c>
@@ -1533,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>3</v>
       </c>
@@ -1553,7 +1552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>3</v>
       </c>
@@ -1573,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>3</v>
       </c>
@@ -1593,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>3</v>
       </c>
@@ -1633,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>3</v>
       </c>
@@ -1653,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>4</v>
       </c>
@@ -1673,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>4</v>
       </c>
@@ -1693,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>4</v>
       </c>
@@ -1713,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>4</v>
       </c>
@@ -1733,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>4</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>4</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>4</v>
       </c>
@@ -1793,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>4</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>4</v>
       </c>
@@ -1833,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>4</v>
       </c>
@@ -1853,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>4</v>
       </c>
@@ -1873,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>4</v>
       </c>
@@ -1893,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>4</v>
       </c>
@@ -1913,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>4</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>4</v>
       </c>
@@ -1953,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>4</v>
       </c>
@@ -1973,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>5</v>
       </c>
@@ -1993,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>5</v>
       </c>
@@ -2013,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>5</v>
       </c>
@@ -2033,7 +2032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>5</v>
       </c>
@@ -2053,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>5</v>
       </c>
@@ -2073,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>5</v>
       </c>
@@ -2093,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>5</v>
       </c>
@@ -2113,7 +2112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>5</v>
       </c>
@@ -2133,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>5</v>
       </c>
@@ -2153,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>5</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>5</v>
       </c>
@@ -2193,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>5</v>
       </c>
@@ -2213,7 +2212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>5</v>
       </c>
@@ -2233,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>5</v>
       </c>
@@ -2253,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>5</v>
       </c>
@@ -2273,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>5</v>
       </c>
@@ -2293,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>0</v>
       </c>
@@ -2307,7 +2306,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>6</v>
       </c>
@@ -2327,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>6</v>
       </c>
@@ -2347,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>6</v>
       </c>
@@ -2367,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>6</v>
       </c>
@@ -2387,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>6</v>
       </c>
@@ -2407,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>6</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>6</v>
       </c>
@@ -2447,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>6</v>
       </c>
@@ -2467,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>6</v>
       </c>
@@ -2487,7 +2486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>6</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>6</v>
       </c>
@@ -2527,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>6</v>
       </c>
@@ -2547,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>6</v>
       </c>
@@ -2567,7 +2566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>6</v>
       </c>
@@ -2587,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>6</v>
       </c>
@@ -2607,7 +2606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>6</v>
       </c>
@@ -2627,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>7</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>7</v>
       </c>
@@ -2667,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>7</v>
       </c>
@@ -2687,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>7</v>
       </c>
@@ -2707,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>7</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>7</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>7</v>
       </c>
@@ -2767,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>7</v>
       </c>
@@ -2787,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>7</v>
       </c>
@@ -2807,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>7</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>7</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>7</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>7</v>
       </c>
@@ -2887,7 +2886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>7</v>
       </c>
@@ -2907,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>7</v>
       </c>
@@ -2927,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>7</v>
       </c>
@@ -2947,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>8</v>
       </c>
@@ -2967,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>8</v>
       </c>
@@ -2987,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>8</v>
       </c>
@@ -3007,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>8</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>8</v>
       </c>
@@ -3047,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>8</v>
       </c>
@@ -3067,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>8</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>8</v>
       </c>
@@ -3107,7 +3106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>8</v>
       </c>
@@ -3127,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>8</v>
       </c>
@@ -3147,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>8</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>8</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>8</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>8</v>
       </c>
@@ -3227,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>8</v>
       </c>
@@ -3247,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>8</v>
       </c>
@@ -3267,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>8</v>
       </c>
@@ -3287,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>9</v>
       </c>
@@ -3307,7 +3306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>9</v>
       </c>
@@ -3327,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>9</v>
       </c>
@@ -3347,7 +3346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>9</v>
       </c>
@@ -3367,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>9</v>
       </c>
@@ -3387,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>9</v>
       </c>
@@ -3407,7 +3406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>9</v>
       </c>
@@ -3427,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>9</v>
       </c>
@@ -3447,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>9</v>
       </c>
@@ -3467,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>9</v>
       </c>
@@ -3487,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>9</v>
       </c>
@@ -3507,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>9</v>
       </c>
@@ -3527,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>9</v>
       </c>
@@ -3547,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>9</v>
       </c>
@@ -3567,7 +3566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>9</v>
       </c>
@@ -3587,7 +3586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>9</v>
       </c>
@@ -3607,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>10</v>
       </c>
@@ -3627,7 +3626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>10</v>
       </c>
@@ -3647,7 +3646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>10</v>
       </c>
@@ -3667,7 +3666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>10</v>
       </c>
@@ -3687,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>10</v>
       </c>
@@ -3707,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>10</v>
       </c>
@@ -3727,7 +3726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>10</v>
       </c>
@@ -3747,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>10</v>
       </c>
@@ -3767,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>10</v>
       </c>
@@ -3787,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>10</v>
       </c>
@@ -3807,7 +3806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>10</v>
       </c>
@@ -3827,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>10</v>
       </c>
@@ -3847,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>10</v>
       </c>
@@ -3867,7 +3866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>10</v>
       </c>
@@ -3887,7 +3886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>10</v>
       </c>
@@ -3907,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>10</v>
       </c>
@@ -3927,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>0</v>
       </c>
@@ -3941,7 +3940,7 @@
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
     </row>
-    <row r="167" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>11</v>
       </c>
@@ -3961,7 +3960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>11</v>
       </c>
@@ -3981,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>11</v>
       </c>
@@ -4001,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>11</v>
       </c>
@@ -4021,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>11</v>
       </c>
@@ -4041,7 +4040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>11</v>
       </c>
@@ -4061,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>11</v>
       </c>
@@ -4081,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>11</v>
       </c>
@@ -4101,7 +4100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>11</v>
       </c>
@@ -4121,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>11</v>
       </c>
@@ -4141,7 +4140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>11</v>
       </c>
@@ -4161,7 +4160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>11</v>
       </c>
@@ -4181,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>11</v>
       </c>
@@ -4201,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>11</v>
       </c>
@@ -4221,7 +4220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>11</v>
       </c>
@@ -4241,7 +4240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>11</v>
       </c>
@@ -4261,7 +4260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>12</v>
       </c>
@@ -4281,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>12</v>
       </c>
@@ -4301,7 +4300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>12</v>
       </c>
@@ -4321,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>12</v>
       </c>
@@ -4341,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>12</v>
       </c>
@@ -4361,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>12</v>
       </c>
@@ -4381,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>12</v>
       </c>
@@ -4401,7 +4400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>12</v>
       </c>
@@ -4421,7 +4420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>12</v>
       </c>
@@ -4441,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>12</v>
       </c>
@@ -4461,7 +4460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>12</v>
       </c>
@@ -4481,7 +4480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>12</v>
       </c>
@@ -4501,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>12</v>
       </c>
@@ -4521,7 +4520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>12</v>
       </c>
@@ -4541,7 +4540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>12</v>
       </c>
@@ -4561,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>12</v>
       </c>
@@ -4581,7 +4580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>12</v>
       </c>
@@ -4601,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>13</v>
       </c>
@@ -4621,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>13</v>
       </c>
@@ -4641,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>13</v>
       </c>
@@ -4661,7 +4660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>13</v>
       </c>
@@ -4681,7 +4680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>13</v>
       </c>
@@ -4701,7 +4700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>13</v>
       </c>
@@ -4721,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>13</v>
       </c>
@@ -4741,7 +4740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>13</v>
       </c>
@@ -4761,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>13</v>
       </c>
@@ -4781,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>13</v>
       </c>
@@ -4801,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>13</v>
       </c>
@@ -4821,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>13</v>
       </c>
@@ -4841,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>13</v>
       </c>
@@ -4861,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>13</v>
       </c>
@@ -4881,7 +4880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>13</v>
       </c>
@@ -4901,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>13</v>
       </c>
@@ -4921,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>14</v>
       </c>
@@ -4941,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>14</v>
       </c>
@@ -4961,7 +4960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>14</v>
       </c>
@@ -4981,7 +4980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>14</v>
       </c>
@@ -5001,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>14</v>
       </c>
@@ -5021,7 +5020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>14</v>
       </c>
@@ -5041,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>14</v>
       </c>
@@ -5061,7 +5060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>14</v>
       </c>
@@ -5081,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>14</v>
       </c>
@@ -5101,7 +5100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>14</v>
       </c>
@@ -5121,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>14</v>
       </c>
@@ -5141,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>14</v>
       </c>
@@ -5161,7 +5160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>14</v>
       </c>
@@ -5181,7 +5180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>14</v>
       </c>
@@ -5201,7 +5200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>14</v>
       </c>
@@ -5221,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>14</v>
       </c>
@@ -5241,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>15</v>
       </c>
@@ -5261,7 +5260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>15</v>
       </c>
@@ -5281,7 +5280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>15</v>
       </c>
@@ -5301,7 +5300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>15</v>
       </c>
@@ -5321,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>15</v>
       </c>
@@ -5341,7 +5340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>15</v>
       </c>
@@ -5361,7 +5360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>15</v>
       </c>
@@ -5381,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>15</v>
       </c>
@@ -5401,7 +5400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>15</v>
       </c>
@@ -5421,7 +5420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>15</v>
       </c>
@@ -5441,7 +5440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>15</v>
       </c>
@@ -5461,7 +5460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>15</v>
       </c>
@@ -5481,7 +5480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>15</v>
       </c>
@@ -5501,7 +5500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>15</v>
       </c>
@@ -5521,7 +5520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>15</v>
       </c>
@@ -5541,7 +5540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>15</v>
       </c>
@@ -5561,7 +5560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>0</v>
       </c>
@@ -5575,7 +5574,7 @@
       <c r="E248" s="1"/>
       <c r="F248" s="1"/>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>16</v>
       </c>
@@ -5595,7 +5594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>16</v>
       </c>
@@ -5615,7 +5614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>16</v>
       </c>
@@ -5635,7 +5634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>16</v>
       </c>
@@ -5655,7 +5654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>16</v>
       </c>
@@ -5675,7 +5674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>16</v>
       </c>
@@ -5695,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>16</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>16</v>
       </c>
@@ -5735,7 +5734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>16</v>
       </c>
@@ -5755,7 +5754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>16</v>
       </c>
@@ -5775,7 +5774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>16</v>
       </c>
@@ -5795,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>16</v>
       </c>
@@ -5815,7 +5814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>16</v>
       </c>
@@ -5835,7 +5834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>16</v>
       </c>
@@ -5855,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>16</v>
       </c>
@@ -5875,7 +5874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>16</v>
       </c>
@@ -5895,7 +5894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>17</v>
       </c>
@@ -5915,7 +5914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>17</v>
       </c>
@@ -5935,7 +5934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>17</v>
       </c>
@@ -5955,7 +5954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>17</v>
       </c>
@@ -5975,7 +5974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>17</v>
       </c>
@@ -5995,7 +5994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>17</v>
       </c>
@@ -6015,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>17</v>
       </c>
@@ -6035,7 +6034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>17</v>
       </c>
@@ -6055,7 +6054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>17</v>
       </c>
@@ -6075,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>17</v>
       </c>
@@ -6095,7 +6094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>17</v>
       </c>
@@ -6115,7 +6114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>17</v>
       </c>
@@ -6135,7 +6134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>17</v>
       </c>
@@ -6155,7 +6154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>17</v>
       </c>
@@ -6175,7 +6174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>17</v>
       </c>
@@ -6195,7 +6194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>17</v>
       </c>
@@ -6215,7 +6214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>17</v>
       </c>
@@ -6235,7 +6234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>18</v>
       </c>
@@ -6255,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>18</v>
       </c>
@@ -6275,7 +6274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>18</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>18</v>
       </c>
@@ -6315,7 +6314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>18</v>
       </c>
@@ -6335,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>18</v>
       </c>
@@ -6355,7 +6354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>18</v>
       </c>
@@ -6375,7 +6374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>18</v>
       </c>
@@ -6395,7 +6394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>18</v>
       </c>
@@ -6415,7 +6414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>18</v>
       </c>
@@ -6435,7 +6434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>18</v>
       </c>
@@ -6455,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>18</v>
       </c>
@@ -6475,7 +6474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>18</v>
       </c>
@@ -6495,7 +6494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>18</v>
       </c>
@@ -6515,7 +6514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>18</v>
       </c>
@@ -6535,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>18</v>
       </c>
@@ -6555,7 +6554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>19</v>
       </c>
@@ -6575,7 +6574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>19</v>
       </c>
@@ -6595,7 +6594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>19</v>
       </c>
@@ -6615,7 +6614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>19</v>
       </c>
@@ -6635,7 +6634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>19</v>
       </c>
@@ -6655,7 +6654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>19</v>
       </c>
@@ -6675,7 +6674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>19</v>
       </c>
@@ -6695,7 +6694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>19</v>
       </c>
@@ -6715,7 +6714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>19</v>
       </c>
@@ -6735,7 +6734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>19</v>
       </c>
@@ -6755,7 +6754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>19</v>
       </c>
@@ -6775,7 +6774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>19</v>
       </c>
@@ -6795,7 +6794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>19</v>
       </c>
@@ -6815,7 +6814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>19</v>
       </c>
@@ -6835,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>19</v>
       </c>
@@ -6855,7 +6854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>19</v>
       </c>
@@ -6875,7 +6874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>20</v>
       </c>
@@ -6895,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>20</v>
       </c>
@@ -6915,7 +6914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>20</v>
       </c>
@@ -6935,7 +6934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>20</v>
       </c>
@@ -6955,7 +6954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>20</v>
       </c>
@@ -6975,7 +6974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>20</v>
       </c>
@@ -6995,7 +6994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>20</v>
       </c>
@@ -7015,7 +7014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>20</v>
       </c>
@@ -7035,7 +7034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>20</v>
       </c>
@@ -7055,7 +7054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>20</v>
       </c>
@@ -7075,7 +7074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>20</v>
       </c>
@@ -7095,7 +7094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>20</v>
       </c>
@@ -7115,7 +7114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>20</v>
       </c>
@@ -7135,7 +7134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>20</v>
       </c>
@@ -7155,7 +7154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>20</v>
       </c>
@@ -7175,7 +7174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>20</v>
       </c>
@@ -7195,7 +7194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>0</v>
       </c>
@@ -7209,7 +7208,7 @@
       <c r="E330" s="1"/>
       <c r="F330" s="1"/>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>21</v>
       </c>
@@ -7229,7 +7228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>21</v>
       </c>
@@ -7249,7 +7248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>21</v>
       </c>
@@ -7269,7 +7268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>21</v>
       </c>
@@ -7289,7 +7288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>21</v>
       </c>
@@ -7309,7 +7308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>21</v>
       </c>
@@ -7329,7 +7328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>21</v>
       </c>
@@ -7349,7 +7348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>21</v>
       </c>
@@ -7369,7 +7368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>21</v>
       </c>
@@ -7389,7 +7388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>21</v>
       </c>
@@ -7409,7 +7408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>21</v>
       </c>
@@ -7429,7 +7428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>21</v>
       </c>
@@ -7449,7 +7448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>21</v>
       </c>
@@ -7469,7 +7468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>21</v>
       </c>
@@ -7489,7 +7488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>21</v>
       </c>
@@ -7509,7 +7508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>21</v>
       </c>
@@ -7529,7 +7528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>22</v>
       </c>
@@ -7549,7 +7548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>22</v>
       </c>
@@ -7569,7 +7568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>22</v>
       </c>
@@ -7589,7 +7588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>22</v>
       </c>
@@ -7609,7 +7608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>22</v>
       </c>
@@ -7629,7 +7628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>22</v>
       </c>
@@ -7649,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>22</v>
       </c>
@@ -7669,7 +7668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>22</v>
       </c>
@@ -7689,7 +7688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>22</v>
       </c>
@@ -7709,7 +7708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>22</v>
       </c>
@@ -7729,7 +7728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>22</v>
       </c>
@@ -7749,7 +7748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>22</v>
       </c>
@@ -7769,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>22</v>
       </c>
@@ -7789,7 +7788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>22</v>
       </c>
@@ -7809,7 +7808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>22</v>
       </c>
@@ -7829,7 +7828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>22</v>
       </c>
@@ -7849,7 +7848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>23</v>
       </c>
@@ -7869,7 +7868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>23</v>
       </c>
@@ -7889,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>23</v>
       </c>
@@ -7909,7 +7908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>23</v>
       </c>
@@ -7929,7 +7928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>23</v>
       </c>
@@ -7949,7 +7948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>23</v>
       </c>
@@ -7969,7 +7968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>23</v>
       </c>
@@ -7989,7 +7988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>23</v>
       </c>
@@ -8009,7 +8008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>23</v>
       </c>
@@ -8029,7 +8028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>23</v>
       </c>
@@ -8049,7 +8048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>23</v>
       </c>
@@ -8069,7 +8068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>23</v>
       </c>
@@ -8089,7 +8088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>23</v>
       </c>
@@ -8109,7 +8108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>23</v>
       </c>
@@ -8129,7 +8128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>23</v>
       </c>
@@ -8149,7 +8148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>23</v>
       </c>
@@ -8169,7 +8168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>23</v>
       </c>
@@ -8189,7 +8188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>24</v>
       </c>
@@ -8209,7 +8208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>24</v>
       </c>
@@ -8229,7 +8228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>24</v>
       </c>
@@ -8249,7 +8248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>24</v>
       </c>
@@ -8269,7 +8268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>24</v>
       </c>
@@ -8289,7 +8288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>24</v>
       </c>
@@ -8309,7 +8308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>24</v>
       </c>
@@ -8329,7 +8328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>24</v>
       </c>
@@ -8349,7 +8348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>24</v>
       </c>
@@ -8369,7 +8368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>24</v>
       </c>
@@ -8389,7 +8388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>24</v>
       </c>
@@ -8409,7 +8408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>24</v>
       </c>
@@ -8429,7 +8428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>24</v>
       </c>
@@ -8449,7 +8448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>24</v>
       </c>
@@ -8469,7 +8468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>24</v>
       </c>
@@ -8489,7 +8488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>24</v>
       </c>
@@ -8509,7 +8508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>25</v>
       </c>
@@ -8529,7 +8528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>25</v>
       </c>
@@ -8549,7 +8548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>25</v>
       </c>
@@ -8569,7 +8568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>25</v>
       </c>
@@ -8589,7 +8588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>25</v>
       </c>
@@ -8609,7 +8608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>25</v>
       </c>
@@ -8629,7 +8628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>25</v>
       </c>
@@ -8649,7 +8648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>25</v>
       </c>
@@ -8669,7 +8668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>25</v>
       </c>
@@ -8689,7 +8688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>25</v>
       </c>
@@ -8709,7 +8708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>25</v>
       </c>
@@ -8729,7 +8728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>25</v>
       </c>
@@ -8749,7 +8748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>25</v>
       </c>
@@ -8769,7 +8768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>25</v>
       </c>
@@ -8789,7 +8788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>25</v>
       </c>
@@ -8809,7 +8808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>25</v>
       </c>
@@ -8829,7 +8828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>0</v>
       </c>

</xml_diff>